<commit_message>
Gantt Chart (not finished)
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfd74915eb265310/Teaching/1810ICT/Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZH\Griffith\Year 5 (2023)\Trimester 2\Software Technologies 2810ICT\Assessments\Assignments\Group project part 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1571A0-8198-41C3-96A9-C503D6380ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9516"/>
+    <workbookView xWindow="3945" yWindow="2715" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -36,90 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>PERIODS</t>
   </si>
   <si>
     <t>ACTIVITY</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -230,41 +153,229 @@
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
     <t>Project Title</t>
+  </si>
+  <si>
+    <t>Define Project Goals and Scope</t>
+  </si>
+  <si>
+    <t>Understand Dataset</t>
+  </si>
+  <si>
+    <t>Form Project Team</t>
+  </si>
+  <si>
+    <r>
+      <t>Project Initiation</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Requirements and Analysis</t>
+  </si>
+  <si>
+    <t>Gather Dataset Details</t>
+  </si>
+  <si>
+    <t>Identify Analysis and Visualization Needs</t>
+  </si>
+  <si>
+    <t>Define Functional and Non-functional Requirements</t>
+  </si>
+  <si>
+    <t>Create Wireframes for User Interface</t>
+  </si>
+  <si>
+    <t>Design User Interaction Flow</t>
+  </si>
+  <si>
+    <t>Define UI Components and Layout</t>
+  </si>
+  <si>
+    <r>
+      <t>User Interface Design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Software Architecture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Select Programming Language and Framework</t>
+  </si>
+  <si>
+    <r>
+      <t>Design System Components (Frontend, Backend):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+  </si>
+  <si>
+    <t>Define Data Storage and Retrieval Approach</t>
+  </si>
+  <si>
+    <r>
+      <t>Implement Data Analysis Features</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Report the information of all listings in a specified suburb</t>
+  </si>
+  <si>
+    <t>Implement chart showing distribution of property prices</t>
+  </si>
+  <si>
+    <t>Retrieve all records containing a user-entered keyword (e.g., pool, pet)</t>
+  </si>
+  <si>
+    <t>Analyse how many customers commented on factors related to cleanliness</t>
+  </si>
+  <si>
+    <t>Implement search by name feature</t>
+  </si>
+  <si>
+    <t>Unit Testing for Individual Components</t>
+  </si>
+  <si>
+    <t>Integration Testing of Modules</t>
+  </si>
+  <si>
+    <t>User Acceptance Testing</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <r>
+      <t>Testing and Quality Assurance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>User Manual Preparation</t>
+  </si>
+  <si>
+    <t>Software Design Document Update</t>
+  </si>
+  <si>
+    <t>Testing Report Compilation</t>
+  </si>
+  <si>
+    <r>
+      <t>Project Management</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Regular Team Meetings and Progress Updates</t>
+  </si>
+  <si>
+    <t>Maintain Git Repository and Version Control</t>
+  </si>
+  <si>
+    <t>Project Review and Finalization</t>
+  </si>
+  <si>
+    <t>Review Project Deliverables</t>
+  </si>
+  <si>
+    <t>Refine User Interface and Functionality</t>
+  </si>
+  <si>
+    <t>Final Testing and Bug Fixing</t>
+  </si>
+  <si>
+    <r>
+      <t>Submission Preparation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1" tint="0.24994659260841701"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Compile Required Documents</t>
+  </si>
+  <si>
+    <t>Review and Ensure Completion</t>
+  </si>
+  <si>
+    <t>Project Submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Part A Submission </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -364,8 +475,54 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF4A66AC"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF4A66AC"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF4A66AC"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,6 +561,23 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,7 +668,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,8 +724,9 @@
     <xf numFmtId="0" fontId="11" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -618,42 +793,48 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="11">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="10" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -666,35 +847,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="10" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="9" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="19" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="19">
-    <cellStyle name="% complete" xfId="16"/>
-    <cellStyle name="% complete (beyond plan) legend" xfId="18"/>
-    <cellStyle name="Activity" xfId="2"/>
-    <cellStyle name="Actual (beyond plan) legend" xfId="17"/>
-    <cellStyle name="Actual legend" xfId="15"/>
+  <cellStyles count="20">
+    <cellStyle name="% complete" xfId="16" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="% complete (beyond plan) legend" xfId="18" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Accent4" xfId="19" builtinId="41"/>
+    <cellStyle name="Activity" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Actual (beyond plan) legend" xfId="17" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Actual legend" xfId="15" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Explanatory Text" xfId="12" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="9" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="10" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="11" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Label" xfId="5"/>
+    <cellStyle name="Label" xfId="5" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Percent Complete" xfId="6"/>
-    <cellStyle name="Period Headers" xfId="3"/>
-    <cellStyle name="Period Highlight Control" xfId="7"/>
-    <cellStyle name="Period Value" xfId="13"/>
-    <cellStyle name="Plan legend" xfId="14"/>
-    <cellStyle name="Project Headers" xfId="4"/>
+    <cellStyle name="Percent Complete" xfId="6" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Period Headers" xfId="3" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Period Highlight Control" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Period Value" xfId="13" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Plan legend" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="49">
     <dxf>
       <fill>
         <patternFill>
@@ -811,6 +1029,34 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
@@ -822,17 +1068,432 @@
           <color theme="9" tint="-0.24994659260841701"/>
         </right>
         <bottom style="thin">
-          <color theme="7"/>
+          <color theme="9" tint="0.59996337778862885"/>
         </bottom>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
-      <border>
-        <top style="thin">
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
           <color theme="7"/>
-        </top>
+        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -1189,33 +1850,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="B1:BO50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
-    <col min="42" max="42" width="2.77734375" customWidth="1"/>
+    <col min="1" max="1" width="2.625" customWidth="1"/>
+    <col min="2" max="2" width="32.75" style="2" customWidth="1"/>
+    <col min="3" max="3" width="11.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="2.75" style="1"/>
+    <col min="42" max="42" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
       <c r="B1" s="14" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
@@ -1223,23 +1884,23 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="24" t="s">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="C2" s="24"/>
       <c r="D2" s="24"/>
       <c r="E2" s="24"/>
       <c r="F2" s="24"/>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>5</v>
       </c>
       <c r="H2" s="15">
         <v>1</v>
       </c>
       <c r="J2" s="16"/>
       <c r="K2" s="30" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="L2" s="31"/>
       <c r="M2" s="31"/>
@@ -1247,58 +1908,58 @@
       <c r="O2" s="32"/>
       <c r="P2" s="17"/>
       <c r="Q2" s="30" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="R2" s="33"/>
       <c r="S2" s="33"/>
       <c r="T2" s="32"/>
       <c r="U2" s="18"/>
-      <c r="V2" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="W2" s="23"/>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="34"/>
+      <c r="V2" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="W2" s="35"/>
+      <c r="X2" s="35"/>
+      <c r="Y2" s="36"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="35" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AA2" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="39"/>
       <c r="AH2" s="20"/>
-      <c r="AI2" s="38" t="s">
-        <v>30</v>
-      </c>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AI2" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="AJ2" s="23"/>
+      <c r="AK2" s="23"/>
+      <c r="AL2" s="23"/>
+      <c r="AM2" s="23"/>
+      <c r="AN2" s="23"/>
+      <c r="AO2" s="23"/>
+      <c r="AP2" s="23"/>
+    </row>
+    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B3" s="25" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>34</v>
+        <v>8</v>
       </c>
       <c r="F3" s="27" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
       <c r="H3" s="21" t="s">
         <v>0</v>
@@ -1323,7 +1984,7 @@
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
       <c r="C4" s="28"/>
       <c r="D4" s="28"/>
@@ -1511,494 +2172,1148 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="7">
+    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="43">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
-        <v>5</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
+      <c r="D5" s="43">
+        <v>4</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="43"/>
+      <c r="G5" s="44">
+        <v>0</v>
+      </c>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+    </row>
+    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="40" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
+    </row>
+    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7">
+        <v>2</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>2</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6" t="s">
+    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="42" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="43">
+        <v>5</v>
+      </c>
+      <c r="D9" s="43">
+        <v>5</v>
+      </c>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
+    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="7">
+        <v>7</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6" t="s">
+    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="7">
         <v>9</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
+      <c r="D12" s="7">
+        <v>2</v>
+      </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="6" t="s">
+    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="43">
         <v>11</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="D13" s="43">
+        <v>6</v>
+      </c>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="41" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="7">
+        <v>11</v>
+      </c>
+      <c r="D14" s="7">
+        <v>2</v>
+      </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="7"/>
+    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="9">
+        <v>13</v>
+      </c>
+      <c r="D15" s="7">
+        <v>2</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
+    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="7">
+        <v>15</v>
+      </c>
+      <c r="D16" s="7">
+        <v>2</v>
+      </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="43">
+        <v>17</v>
+      </c>
+      <c r="D17" s="43">
+        <v>5</v>
+      </c>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="40" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="7">
+        <v>17</v>
+      </c>
+      <c r="D18" s="7">
+        <v>1</v>
+      </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="7">
+        <v>18</v>
+      </c>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
       <c r="G19" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="7">
+        <v>21</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1</v>
+      </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="6" t="s">
-        <v>18</v>
+    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="40" t="s">
+        <v>56</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
-      <c r="G21" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
+      <c r="G21" s="8"/>
+    </row>
+    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="43">
+        <v>22</v>
+      </c>
+      <c r="D22" s="43">
+        <v>15</v>
+      </c>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="40" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="7">
+        <v>22</v>
+      </c>
+      <c r="D23" s="7">
+        <v>3</v>
+      </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
+    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="40" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="7">
+        <v>25</v>
+      </c>
+      <c r="D24" s="7">
+        <v>2</v>
+      </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
       <c r="G24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
+    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="7">
+        <v>27</v>
+      </c>
+      <c r="D25" s="7">
+        <v>2</v>
+      </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="7">
+        <v>29</v>
+      </c>
+      <c r="D26" s="7">
+        <v>3</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="7">
+        <v>32</v>
+      </c>
+      <c r="D27" s="7">
+        <v>5</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
+    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C28" s="43">
+        <v>37</v>
+      </c>
+      <c r="D28" s="43">
+        <v>8</v>
+      </c>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="7">
+        <v>37</v>
+      </c>
+      <c r="D29" s="7">
+        <v>3</v>
+      </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
       <c r="G29" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
+    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="7">
+        <v>40</v>
+      </c>
+      <c r="D30" s="7">
+        <v>3</v>
+      </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+    <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="7">
+        <v>43</v>
+      </c>
+      <c r="D31" s="7">
+        <v>2</v>
+      </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B33" s="6" t="s">
+    <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="C32" s="43">
+        <v>45</v>
+      </c>
+      <c r="D32" s="43">
+        <v>5</v>
+      </c>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
+      <c r="C33" s="7">
+        <v>45</v>
+      </c>
+      <c r="D33" s="7">
+        <v>2</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="6" t="s">
+    <row r="34" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="C34" s="7">
+        <v>47</v>
+      </c>
+      <c r="D34" s="7">
+        <v>2</v>
+      </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
       <c r="G34" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B35" s="6" t="s">
+    <row r="35" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
+      <c r="C35" s="7">
+        <v>49</v>
+      </c>
+      <c r="D35" s="7">
+        <v>1</v>
+      </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
       <c r="G35" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="6" t="s">
+    <row r="36" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="6" t="s">
+      <c r="C36" s="43">
+        <v>50</v>
+      </c>
+      <c r="D36" s="43">
+        <v>2</v>
+      </c>
+      <c r="E36" s="43"/>
+      <c r="F36" s="43"/>
+      <c r="G36" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="C37" s="7">
+        <v>52</v>
+      </c>
+      <c r="D37" s="7">
+        <v>1</v>
+      </c>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="6" t="s">
+    <row r="38" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
+      <c r="C38" s="7">
+        <v>53</v>
+      </c>
+      <c r="D38" s="7">
+        <v>1</v>
+      </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="6" t="s">
+    <row r="39" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="46" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="7"/>
-      <c r="E39" s="7"/>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
+      <c r="C39" s="43">
+        <v>53</v>
+      </c>
+      <c r="D39" s="43">
+        <v>5</v>
+      </c>
+      <c r="E39" s="43"/>
+      <c r="F39" s="43"/>
+      <c r="G39" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="7">
+        <v>53</v>
+      </c>
+      <c r="D40" s="7">
+        <v>2</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="7">
+        <v>55</v>
+      </c>
+      <c r="D41" s="7">
+        <v>2</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="7">
+        <v>57</v>
+      </c>
+      <c r="D42" s="7">
+        <v>1</v>
+      </c>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="46" t="s">
+        <v>52</v>
+      </c>
+      <c r="C43" s="43">
+        <v>58</v>
+      </c>
+      <c r="D43" s="43">
+        <v>3</v>
+      </c>
+      <c r="E43" s="43"/>
+      <c r="F43" s="43"/>
+      <c r="G43" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C44" s="7">
+        <v>58</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1</v>
+      </c>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="7">
+        <v>59</v>
+      </c>
+      <c r="D45" s="7">
+        <v>1</v>
+      </c>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="50">
+        <v>60</v>
+      </c>
+      <c r="D46" s="50">
+        <v>1</v>
+      </c>
+      <c r="E46" s="50"/>
+      <c r="F46" s="50"/>
+      <c r="G46" s="51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="48"/>
+      <c r="I47" s="48"/>
+      <c r="J47" s="48"/>
+      <c r="K47" s="48"/>
+      <c r="L47" s="48"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="48"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="48"/>
+      <c r="R47" s="48"/>
+      <c r="S47" s="48"/>
+      <c r="T47" s="48"/>
+      <c r="U47" s="48"/>
+      <c r="V47" s="48"/>
+      <c r="W47" s="48"/>
+      <c r="X47" s="48"/>
+      <c r="Y47" s="48"/>
+      <c r="Z47" s="48"/>
+      <c r="AA47" s="48"/>
+      <c r="AB47" s="49"/>
+      <c r="AC47" s="49"/>
+      <c r="AD47" s="49"/>
+      <c r="AE47" s="49"/>
+      <c r="AF47" s="49"/>
+      <c r="AG47" s="49"/>
+      <c r="AH47" s="49"/>
+      <c r="AI47" s="49"/>
+      <c r="AJ47" s="49"/>
+      <c r="AK47" s="49"/>
+      <c r="AL47" s="49"/>
+      <c r="AM47" s="49"/>
+      <c r="AN47" s="49"/>
+      <c r="AO47" s="49"/>
+      <c r="AP47" s="49"/>
+      <c r="AQ47" s="49"/>
+      <c r="AR47" s="49"/>
+      <c r="AS47" s="49"/>
+      <c r="AT47" s="49"/>
+      <c r="AU47" s="49"/>
+      <c r="AV47" s="49"/>
+      <c r="AW47" s="49"/>
+      <c r="AX47" s="49"/>
+      <c r="AY47" s="49"/>
+      <c r="AZ47" s="49"/>
+      <c r="BA47" s="49"/>
+      <c r="BB47" s="49"/>
+      <c r="BC47" s="49"/>
+      <c r="BD47" s="49"/>
+      <c r="BE47" s="49"/>
+      <c r="BF47" s="49"/>
+      <c r="BG47" s="49"/>
+      <c r="BH47" s="49"/>
+      <c r="BI47" s="49"/>
+      <c r="BJ47" s="49"/>
+      <c r="BK47" s="49"/>
+      <c r="BL47" s="49"/>
+      <c r="BM47" s="49"/>
+      <c r="BN47" s="49"/>
+      <c r="BO47" s="49"/>
+    </row>
+    <row r="48" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="48"/>
+      <c r="I48" s="48"/>
+      <c r="J48" s="48"/>
+      <c r="K48" s="48"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="48"/>
+      <c r="P48" s="48"/>
+      <c r="Q48" s="48"/>
+      <c r="R48" s="48"/>
+      <c r="S48" s="48"/>
+      <c r="T48" s="48"/>
+      <c r="U48" s="48"/>
+      <c r="V48" s="48"/>
+      <c r="W48" s="48"/>
+      <c r="X48" s="48"/>
+      <c r="Y48" s="48"/>
+      <c r="Z48" s="48"/>
+      <c r="AA48" s="48"/>
+      <c r="AB48" s="49"/>
+      <c r="AC48" s="49"/>
+      <c r="AD48" s="49"/>
+      <c r="AE48" s="49"/>
+      <c r="AF48" s="49"/>
+      <c r="AG48" s="49"/>
+      <c r="AH48" s="49"/>
+      <c r="AI48" s="49"/>
+      <c r="AJ48" s="49"/>
+      <c r="AK48" s="49"/>
+      <c r="AL48" s="49"/>
+      <c r="AM48" s="49"/>
+      <c r="AN48" s="49"/>
+      <c r="AO48" s="49"/>
+      <c r="AP48" s="49"/>
+      <c r="AQ48" s="49"/>
+      <c r="AR48" s="49"/>
+      <c r="AS48" s="49"/>
+      <c r="AT48" s="49"/>
+      <c r="AU48" s="49"/>
+      <c r="AV48" s="49"/>
+      <c r="AW48" s="49"/>
+      <c r="AX48" s="49"/>
+      <c r="AY48" s="49"/>
+      <c r="AZ48" s="49"/>
+      <c r="BA48" s="49"/>
+      <c r="BB48" s="49"/>
+      <c r="BC48" s="49"/>
+      <c r="BD48" s="49"/>
+      <c r="BE48" s="49"/>
+      <c r="BF48" s="49"/>
+      <c r="BG48" s="49"/>
+      <c r="BH48" s="49"/>
+      <c r="BI48" s="49"/>
+      <c r="BJ48" s="49"/>
+      <c r="BK48" s="49"/>
+      <c r="BL48" s="49"/>
+      <c r="BM48" s="49"/>
+      <c r="BN48" s="49"/>
+      <c r="BO48" s="49"/>
+    </row>
+    <row r="49" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="48"/>
+      <c r="I49" s="48"/>
+      <c r="J49" s="48"/>
+      <c r="K49" s="48"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="48"/>
+      <c r="R49" s="48"/>
+      <c r="S49" s="48"/>
+      <c r="T49" s="48"/>
+      <c r="U49" s="48"/>
+      <c r="V49" s="48"/>
+      <c r="W49" s="48"/>
+      <c r="X49" s="48"/>
+      <c r="Y49" s="48"/>
+      <c r="Z49" s="48"/>
+      <c r="AA49" s="48"/>
+      <c r="AB49" s="49"/>
+      <c r="AC49" s="49"/>
+      <c r="AD49" s="49"/>
+      <c r="AE49" s="49"/>
+      <c r="AF49" s="49"/>
+      <c r="AG49" s="49"/>
+      <c r="AH49" s="49"/>
+      <c r="AI49" s="49"/>
+      <c r="AJ49" s="49"/>
+      <c r="AK49" s="49"/>
+      <c r="AL49" s="49"/>
+      <c r="AM49" s="49"/>
+      <c r="AN49" s="49"/>
+      <c r="AO49" s="49"/>
+      <c r="AP49" s="49"/>
+      <c r="AQ49" s="49"/>
+      <c r="AR49" s="49"/>
+      <c r="AS49" s="49"/>
+      <c r="AT49" s="49"/>
+      <c r="AU49" s="49"/>
+      <c r="AV49" s="49"/>
+      <c r="AW49" s="49"/>
+      <c r="AX49" s="49"/>
+      <c r="AY49" s="49"/>
+      <c r="AZ49" s="49"/>
+      <c r="BA49" s="49"/>
+      <c r="BB49" s="49"/>
+      <c r="BC49" s="49"/>
+      <c r="BD49" s="49"/>
+      <c r="BE49" s="49"/>
+      <c r="BF49" s="49"/>
+      <c r="BG49" s="49"/>
+      <c r="BH49" s="49"/>
+      <c r="BI49" s="49"/>
+      <c r="BJ49" s="49"/>
+      <c r="BK49" s="49"/>
+      <c r="BL49" s="49"/>
+      <c r="BM49" s="49"/>
+      <c r="BN49" s="49"/>
+      <c r="BO49" s="49"/>
+    </row>
+    <row r="50" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+      <c r="J50" s="48"/>
+      <c r="K50" s="48"/>
+      <c r="L50" s="48"/>
+      <c r="M50" s="48"/>
+      <c r="N50" s="48"/>
+      <c r="O50" s="48"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
+      <c r="S50" s="48"/>
+      <c r="T50" s="48"/>
+      <c r="U50" s="48"/>
+      <c r="V50" s="48"/>
+      <c r="W50" s="48"/>
+      <c r="X50" s="48"/>
+      <c r="Y50" s="48"/>
+      <c r="Z50" s="48"/>
+      <c r="AA50" s="48"/>
+      <c r="AB50" s="49"/>
+      <c r="AC50" s="49"/>
+      <c r="AD50" s="49"/>
+      <c r="AE50" s="49"/>
+      <c r="AF50" s="49"/>
+      <c r="AG50" s="49"/>
+      <c r="AH50" s="49"/>
+      <c r="AI50" s="49"/>
+      <c r="AJ50" s="49"/>
+      <c r="AK50" s="49"/>
+      <c r="AL50" s="49"/>
+      <c r="AM50" s="49"/>
+      <c r="AN50" s="49"/>
+      <c r="AO50" s="49"/>
+      <c r="AP50" s="49"/>
+      <c r="AQ50" s="49"/>
+      <c r="AR50" s="49"/>
+      <c r="AS50" s="49"/>
+      <c r="AT50" s="49"/>
+      <c r="AU50" s="49"/>
+      <c r="AV50" s="49"/>
+      <c r="AW50" s="49"/>
+      <c r="AX50" s="49"/>
+      <c r="AY50" s="49"/>
+      <c r="AZ50" s="49"/>
+      <c r="BA50" s="49"/>
+      <c r="BB50" s="49"/>
+      <c r="BC50" s="49"/>
+      <c r="BD50" s="49"/>
+      <c r="BE50" s="49"/>
+      <c r="BF50" s="49"/>
+      <c r="BG50" s="49"/>
+      <c r="BH50" s="49"/>
+      <c r="BI50" s="49"/>
+      <c r="BJ50" s="49"/>
+      <c r="BK50" s="49"/>
+      <c r="BL50" s="49"/>
+      <c r="BM50" s="49"/>
+      <c r="BN50" s="49"/>
+      <c r="BO50" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO39">
-    <cfRule type="expression" dxfId="17" priority="1">
+  <conditionalFormatting sqref="H5:BO40">
+    <cfRule type="expression" dxfId="48" priority="41">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="3">
+    <cfRule type="expression" dxfId="47" priority="43">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="4">
+    <cfRule type="expression" dxfId="46" priority="44">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="45" priority="45">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="44" priority="46">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="43" priority="47">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="11">
+    <cfRule type="expression" dxfId="42" priority="51">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="12">
+    <cfRule type="expression" dxfId="41" priority="52">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:BO4">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="40" priority="48">
       <formula>H$4=period_selected</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H41:BO42">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H43:BO44">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:BO46">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47:BO48">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H49:BO50">
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="4">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Gantt implementation (Ready for Submission)
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26827"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZH\Griffith\Year 5 (2023)\Trimester 2\Software Technologies 2810ICT\Assessments\Assignments\Group project part 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ZH\Griffith\Year 5 (2023)\Trimester 2\Software Technologies 2810ICT\Assessments\Assignments\Group Project Part 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E84F9DE-4ACC-42E9-AA1D-AC5981C0DFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383CA0CD-65CB-4079-800E-1A7BE3DDE225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,19 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -829,6 +840,30 @@
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="19" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="9" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="10" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -867,30 +902,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="11" borderId="0" xfId="6" applyFont="1" applyFill="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="9" borderId="2" xfId="6" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="20">
@@ -1408,8 +1419,8 @@
   </sheetPr>
   <dimension ref="A1:BO50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z1" sqref="Z1"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1436,13 +1447,13 @@
       <c r="G1" s="12"/>
     </row>
     <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
       <c r="G2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1450,37 +1461,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="15"/>
-      <c r="K2" s="36" t="s">
+      <c r="K2" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="46"/>
       <c r="P2" s="16"/>
-      <c r="Q2" s="36" t="s">
+      <c r="Q2" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="38"/>
+      <c r="R2" s="47"/>
+      <c r="S2" s="47"/>
+      <c r="T2" s="46"/>
       <c r="U2" s="17"/>
-      <c r="V2" s="40" t="s">
+      <c r="V2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="W2" s="41"/>
-      <c r="X2" s="41"/>
-      <c r="Y2" s="42"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="50"/>
       <c r="Z2" s="18"/>
-      <c r="AA2" s="40" t="s">
+      <c r="AA2" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="41"/>
-      <c r="AC2" s="41"/>
-      <c r="AD2" s="41"/>
-      <c r="AE2" s="41"/>
-      <c r="AF2" s="41"/>
-      <c r="AG2" s="42"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="50"/>
       <c r="AH2" s="19"/>
       <c r="AI2" s="21" t="s">
         <v>4</v>
@@ -1494,22 +1505,22 @@
       <c r="AP2" s="22"/>
     </row>
     <row r="3" spans="2:67" s="11" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="52" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="46" t="s">
+      <c r="E3" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="46" t="s">
+      <c r="F3" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="42" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="20" t="s">
@@ -1536,12 +1547,12 @@
       <c r="AA3" s="10"/>
     </row>
     <row r="4" spans="2:67" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="45"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1919,9 +1930,9 @@
       <c r="D13" s="6">
         <v>1</v>
       </c>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="48">
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35">
         <v>1</v>
       </c>
       <c r="T13" s="18"/>
@@ -1996,7 +2007,7 @@
       <c r="Y16" s="18"/>
       <c r="Z16" s="19"/>
     </row>
-    <row r="17" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="24" t="s">
         <v>22</v>
       </c>
@@ -2017,7 +2028,7 @@
       <c r="Y17" s="19"/>
       <c r="Z17"/>
     </row>
-    <row r="18" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="24" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2048,7 @@
       <c r="Y18" s="19"/>
       <c r="Z18"/>
     </row>
-    <row r="19" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="24" t="s">
         <v>24</v>
       </c>
@@ -2056,7 +2067,7 @@
       <c r="Y19" s="18"/>
       <c r="Z19" s="19"/>
     </row>
-    <row r="20" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="29" t="s">
         <v>26</v>
       </c>
@@ -2077,7 +2088,7 @@
       <c r="Z20" s="16"/>
       <c r="AA20" s="16"/>
     </row>
-    <row r="21" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
         <v>27</v>
       </c>
@@ -2096,7 +2107,7 @@
       <c r="Y21" s="18"/>
       <c r="Z21" s="19"/>
     </row>
-    <row r="22" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>28</v>
       </c>
@@ -2106,16 +2117,16 @@
       <c r="D22" s="6">
         <v>3</v>
       </c>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-      <c r="G22" s="48">
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="35">
         <v>1</v>
       </c>
       <c r="X22" s="16"/>
       <c r="Y22" s="16"/>
       <c r="Z22" s="17"/>
     </row>
-    <row r="23" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
         <v>29</v>
       </c>
@@ -2125,14 +2136,14 @@
       <c r="D23" s="6">
         <v>1</v>
       </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="48">
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="35">
         <v>1</v>
       </c>
       <c r="AA23" s="17"/>
     </row>
-    <row r="24" spans="2:28" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="23" t="s">
         <v>55</v>
       </c>
@@ -2142,15 +2153,15 @@
       <c r="D24" s="6">
         <v>2</v>
       </c>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-      <c r="G24" s="48">
+      <c r="E24" s="34"/>
+      <c r="F24" s="34"/>
+      <c r="G24" s="35">
         <v>0.5</v>
       </c>
       <c r="AA24" s="16"/>
-      <c r="AB24" s="1"/>
-    </row>
-    <row r="25" spans="2:28" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AB24" s="17"/>
+    </row>
+    <row r="25" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="30" t="s">
         <v>30</v>
       </c>
@@ -2163,10 +2174,12 @@
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
       <c r="G25" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BJ25" s="18"/>
+      <c r="BK25" s="19"/>
+    </row>
+    <row r="26" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>31</v>
       </c>
@@ -2176,13 +2189,14 @@
       <c r="D26" s="6">
         <v>3</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="34"/>
+      <c r="F26" s="34"/>
+      <c r="G26" s="35">
+        <v>1</v>
+      </c>
+      <c r="BJ26" s="19"/>
+    </row>
+    <row r="27" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>32</v>
       </c>
@@ -2192,13 +2206,14 @@
       <c r="D27" s="6">
         <v>2</v>
       </c>
-      <c r="E27" s="47"/>
-      <c r="F27" s="47"/>
-      <c r="G27" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="G27" s="35">
+        <v>1</v>
+      </c>
+      <c r="BK27" s="19"/>
+    </row>
+    <row r="28" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>33</v>
       </c>
@@ -2208,13 +2223,14 @@
       <c r="D28" s="6">
         <v>2</v>
       </c>
-      <c r="E28" s="47"/>
-      <c r="F28" s="47"/>
-      <c r="G28" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="35">
+        <v>1</v>
+      </c>
+      <c r="BJ28" s="19"/>
+    </row>
+    <row r="29" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
         <v>34</v>
       </c>
@@ -2224,13 +2240,14 @@
       <c r="D29" s="6">
         <v>3</v>
       </c>
-      <c r="E29" s="47"/>
-      <c r="F29" s="47"/>
-      <c r="G29" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="35">
+        <v>1</v>
+      </c>
+      <c r="BJ29" s="19"/>
+    </row>
+    <row r="30" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="24" t="s">
         <v>35</v>
       </c>
@@ -2240,13 +2257,14 @@
       <c r="D30" s="6">
         <v>5</v>
       </c>
-      <c r="E30" s="47"/>
-      <c r="F30" s="47"/>
-      <c r="G30" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="35">
+        <v>1</v>
+      </c>
+      <c r="BJ30" s="19"/>
+    </row>
+    <row r="31" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="28" t="s">
         <v>40</v>
       </c>
@@ -2259,10 +2277,16 @@
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BJ31" s="18"/>
+      <c r="BK31" s="18"/>
+      <c r="BL31" s="18"/>
+      <c r="BM31" s="18"/>
+      <c r="BN31" s="18"/>
+      <c r="BO31" s="19"/>
+    </row>
+    <row r="32" spans="2:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="24" t="s">
         <v>36</v>
       </c>
@@ -2272,13 +2296,19 @@
       <c r="D32" s="6">
         <v>3</v>
       </c>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="BJ32" s="18"/>
+      <c r="BK32" s="18"/>
+      <c r="BL32" s="18"/>
+      <c r="BM32" s="18"/>
+      <c r="BN32" s="18"/>
+      <c r="BO32" s="19"/>
+    </row>
+    <row r="33" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="24" t="s">
         <v>37</v>
       </c>
@@ -2288,13 +2318,16 @@
       <c r="D33" s="6">
         <v>3</v>
       </c>
-      <c r="E33" s="47"/>
-      <c r="F33" s="47"/>
-      <c r="G33" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="35">
+        <v>0.8</v>
+      </c>
+      <c r="BM33" s="18"/>
+      <c r="BN33" s="18"/>
+      <c r="BO33" s="19"/>
+    </row>
+    <row r="34" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="24" t="s">
         <v>38</v>
       </c>
@@ -2304,13 +2337,15 @@
       <c r="D34" s="6">
         <v>2</v>
       </c>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="35">
+        <v>1</v>
+      </c>
+      <c r="BN34" s="18"/>
+      <c r="BO34" s="19"/>
+    </row>
+    <row r="35" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="29" t="s">
         <v>39</v>
       </c>
@@ -2323,10 +2358,12 @@
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
       <c r="G35" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BN35" s="18"/>
+      <c r="BO35" s="19"/>
+    </row>
+    <row r="36" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="24" t="s">
         <v>41</v>
       </c>
@@ -2336,13 +2373,14 @@
       <c r="D36" s="6">
         <v>2</v>
       </c>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E36" s="34"/>
+      <c r="F36" s="34"/>
+      <c r="G36" s="35">
+        <v>1</v>
+      </c>
+      <c r="BO36" s="19"/>
+    </row>
+    <row r="37" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B37" s="24" t="s">
         <v>42</v>
       </c>
@@ -2352,13 +2390,14 @@
       <c r="D37" s="6">
         <v>2</v>
       </c>
-      <c r="E37" s="47"/>
-      <c r="F37" s="47"/>
-      <c r="G37" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E37" s="34"/>
+      <c r="F37" s="34"/>
+      <c r="G37" s="35">
+        <v>1</v>
+      </c>
+      <c r="BO37" s="19"/>
+    </row>
+    <row r="38" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B38" s="24" t="s">
         <v>43</v>
       </c>
@@ -2371,10 +2410,11 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BO38" s="19"/>
+    </row>
+    <row r="39" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B39" s="29" t="s">
         <v>47</v>
       </c>
@@ -2387,10 +2427,16 @@
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
       <c r="G39" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BJ39" s="16"/>
+      <c r="BK39" s="16"/>
+      <c r="BL39" s="16"/>
+      <c r="BM39" s="18"/>
+      <c r="BN39" s="18"/>
+      <c r="BO39" s="19"/>
+    </row>
+    <row r="40" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="24" t="s">
         <v>48</v>
       </c>
@@ -2403,10 +2449,11 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BO40" s="19"/>
+    </row>
+    <row r="41" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="24" t="s">
         <v>49</v>
       </c>
@@ -2419,10 +2466,13 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BM41" s="18"/>
+      <c r="BN41" s="18"/>
+      <c r="BO41" s="19"/>
+    </row>
+    <row r="42" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="24" t="s">
         <v>50</v>
       </c>
@@ -2435,10 +2485,14 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BL42" s="16"/>
+      <c r="BM42" s="18"/>
+      <c r="BN42" s="18"/>
+      <c r="BO42" s="19"/>
+    </row>
+    <row r="43" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="29" t="s">
         <v>51</v>
       </c>
@@ -2451,10 +2505,11 @@
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
       <c r="G43" s="27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BO43" s="17"/>
+    </row>
+    <row r="44" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="24" t="s">
         <v>52</v>
       </c>
@@ -2467,10 +2522,11 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="BO44" s="19"/>
+    </row>
+    <row r="45" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="24" t="s">
         <v>53</v>
       </c>
@@ -2483,154 +2539,155 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="50"/>
-      <c r="B46" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="BO45" s="19"/>
+    </row>
+    <row r="46" spans="1:67" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="37"/>
+      <c r="B46" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C46" s="52">
+      <c r="C46" s="39">
         <v>60</v>
       </c>
-      <c r="D46" s="52">
-        <v>1</v>
-      </c>
-      <c r="E46" s="52"/>
-      <c r="F46" s="52"/>
-      <c r="G46" s="53">
-        <v>0</v>
-      </c>
-      <c r="H46" s="54"/>
-      <c r="I46" s="54"/>
-      <c r="J46" s="54"/>
-      <c r="K46" s="54"/>
-      <c r="L46" s="54"/>
-      <c r="M46" s="54"/>
-      <c r="N46" s="54"/>
-      <c r="O46" s="54"/>
-      <c r="P46" s="54"/>
-      <c r="Q46" s="54"/>
-      <c r="R46" s="54"/>
-      <c r="S46" s="54"/>
-      <c r="T46" s="54"/>
-      <c r="U46" s="54"/>
-      <c r="V46" s="54"/>
-      <c r="W46" s="54"/>
-      <c r="X46" s="54"/>
-      <c r="Y46" s="54"/>
-      <c r="Z46" s="54"/>
-      <c r="AA46" s="54"/>
-      <c r="AB46" s="50"/>
-      <c r="AC46" s="50"/>
-      <c r="AD46" s="50"/>
-      <c r="AE46" s="50"/>
-      <c r="AF46" s="50"/>
-      <c r="AG46" s="50"/>
-      <c r="AH46" s="50"/>
-      <c r="AI46" s="50"/>
-      <c r="AJ46" s="50"/>
-      <c r="AK46" s="50"/>
-      <c r="AL46" s="50"/>
-      <c r="AM46" s="50"/>
-      <c r="AN46" s="50"/>
-      <c r="AO46" s="50"/>
-      <c r="AP46" s="50"/>
-      <c r="AQ46" s="50"/>
-      <c r="AR46" s="50"/>
-      <c r="AS46" s="50"/>
-      <c r="AT46" s="50"/>
-      <c r="AU46" s="50"/>
-      <c r="AV46" s="50"/>
-      <c r="AW46" s="50"/>
-      <c r="AX46" s="50"/>
-      <c r="AY46" s="50"/>
-      <c r="AZ46" s="50"/>
-      <c r="BA46" s="50"/>
-      <c r="BB46" s="50"/>
-      <c r="BC46" s="50"/>
-      <c r="BD46" s="50"/>
-      <c r="BE46" s="50"/>
-      <c r="BF46" s="50"/>
-      <c r="BG46" s="50"/>
-      <c r="BH46" s="50"/>
-      <c r="BI46" s="50"/>
-      <c r="BJ46" s="50"/>
-      <c r="BK46" s="50"/>
-      <c r="BL46" s="50"/>
-      <c r="BM46" s="50"/>
-      <c r="BN46" s="50"/>
-      <c r="BO46" s="50"/>
-    </row>
-    <row r="47" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="49"/>
-      <c r="B47" s="49"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
-      <c r="E47" s="49"/>
-      <c r="F47" s="49"/>
-      <c r="G47" s="49"/>
-      <c r="H47" s="49"/>
-      <c r="I47" s="49"/>
-      <c r="J47" s="49"/>
-      <c r="K47" s="49"/>
-      <c r="L47" s="49"/>
-      <c r="M47" s="49"/>
-      <c r="N47" s="49"/>
-      <c r="O47" s="49"/>
-      <c r="P47" s="49"/>
-      <c r="Q47" s="49"/>
-      <c r="R47" s="49"/>
-      <c r="S47" s="49"/>
-      <c r="T47" s="49"/>
-      <c r="U47" s="49"/>
-      <c r="V47" s="49"/>
-      <c r="W47" s="49"/>
-      <c r="X47" s="49"/>
-      <c r="Y47" s="49"/>
-      <c r="Z47" s="49"/>
-      <c r="AA47" s="49"/>
-      <c r="AB47" s="49"/>
-      <c r="AC47" s="49"/>
-      <c r="AD47" s="49"/>
-      <c r="AE47" s="49"/>
-      <c r="AF47" s="49"/>
-      <c r="AG47" s="49"/>
-      <c r="AH47" s="49"/>
-      <c r="AI47" s="49"/>
-      <c r="AJ47" s="49"/>
-      <c r="AK47" s="49"/>
-      <c r="AL47" s="49"/>
-      <c r="AM47" s="49"/>
-      <c r="AN47" s="49"/>
-      <c r="AO47" s="49"/>
-      <c r="AP47" s="49"/>
-      <c r="AQ47" s="49"/>
-      <c r="AR47" s="49"/>
-      <c r="AS47" s="49"/>
-      <c r="AT47" s="49"/>
-      <c r="AU47" s="49"/>
-      <c r="AV47" s="49"/>
-      <c r="AW47" s="49"/>
-      <c r="AX47" s="49"/>
-      <c r="AY47" s="49"/>
-      <c r="AZ47" s="49"/>
-      <c r="BA47" s="49"/>
-      <c r="BB47" s="49"/>
-      <c r="BC47" s="49"/>
-      <c r="BD47" s="49"/>
-      <c r="BE47" s="49"/>
-      <c r="BF47" s="49"/>
-      <c r="BG47" s="49"/>
-      <c r="BH47" s="49"/>
-      <c r="BI47" s="49"/>
-      <c r="BJ47" s="49"/>
-      <c r="BK47" s="49"/>
-      <c r="BL47" s="49"/>
-      <c r="BM47" s="49"/>
-      <c r="BN47" s="49"/>
-      <c r="BO47" s="49"/>
+      <c r="D46" s="39">
+        <v>1</v>
+      </c>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="40">
+        <v>1</v>
+      </c>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="41"/>
+      <c r="K46" s="41"/>
+      <c r="L46" s="41"/>
+      <c r="M46" s="41"/>
+      <c r="N46" s="41"/>
+      <c r="O46" s="41"/>
+      <c r="P46" s="41"/>
+      <c r="Q46" s="41"/>
+      <c r="R46" s="41"/>
+      <c r="S46" s="41"/>
+      <c r="T46" s="41"/>
+      <c r="U46" s="41"/>
+      <c r="V46" s="41"/>
+      <c r="W46" s="41"/>
+      <c r="X46" s="41"/>
+      <c r="Y46" s="41"/>
+      <c r="Z46" s="41"/>
+      <c r="AA46" s="41"/>
+      <c r="AB46" s="37"/>
+      <c r="AC46" s="37"/>
+      <c r="AD46" s="37"/>
+      <c r="AE46" s="37"/>
+      <c r="AF46" s="37"/>
+      <c r="AG46" s="37"/>
+      <c r="AH46" s="37"/>
+      <c r="AI46" s="37"/>
+      <c r="AJ46" s="37"/>
+      <c r="AK46" s="37"/>
+      <c r="AL46" s="37"/>
+      <c r="AM46" s="37"/>
+      <c r="AN46" s="37"/>
+      <c r="AO46" s="37"/>
+      <c r="AP46" s="37"/>
+      <c r="AQ46" s="37"/>
+      <c r="AR46" s="37"/>
+      <c r="AS46" s="37"/>
+      <c r="AT46" s="37"/>
+      <c r="AU46" s="37"/>
+      <c r="AV46" s="37"/>
+      <c r="AW46" s="37"/>
+      <c r="AX46" s="37"/>
+      <c r="AY46" s="37"/>
+      <c r="AZ46" s="37"/>
+      <c r="BA46" s="37"/>
+      <c r="BB46" s="37"/>
+      <c r="BC46" s="37"/>
+      <c r="BD46" s="37"/>
+      <c r="BE46" s="37"/>
+      <c r="BF46" s="37"/>
+      <c r="BG46" s="37"/>
+      <c r="BH46" s="37"/>
+      <c r="BI46" s="37"/>
+      <c r="BJ46" s="37"/>
+      <c r="BK46" s="37"/>
+      <c r="BL46" s="37"/>
+      <c r="BM46" s="37"/>
+      <c r="BN46" s="37"/>
+      <c r="BO46" s="17"/>
+    </row>
+    <row r="47" spans="1:67" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="36"/>
+      <c r="E47" s="36"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="36"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
+      <c r="K47" s="36"/>
+      <c r="L47" s="36"/>
+      <c r="M47" s="36"/>
+      <c r="N47" s="36"/>
+      <c r="O47" s="36"/>
+      <c r="P47" s="36"/>
+      <c r="Q47" s="36"/>
+      <c r="R47" s="36"/>
+      <c r="S47" s="36"/>
+      <c r="T47" s="36"/>
+      <c r="U47" s="36"/>
+      <c r="V47" s="36"/>
+      <c r="W47" s="36"/>
+      <c r="X47" s="36"/>
+      <c r="Y47" s="36"/>
+      <c r="Z47" s="36"/>
+      <c r="AA47" s="36"/>
+      <c r="AB47" s="36"/>
+      <c r="AC47" s="36"/>
+      <c r="AD47" s="36"/>
+      <c r="AE47" s="36"/>
+      <c r="AF47" s="36"/>
+      <c r="AG47" s="36"/>
+      <c r="AH47" s="36"/>
+      <c r="AI47" s="36"/>
+      <c r="AJ47" s="36"/>
+      <c r="AK47" s="36"/>
+      <c r="AL47" s="36"/>
+      <c r="AM47" s="36"/>
+      <c r="AN47" s="36"/>
+      <c r="AO47" s="36"/>
+      <c r="AP47" s="36"/>
+      <c r="AQ47" s="36"/>
+      <c r="AR47" s="36"/>
+      <c r="AS47" s="36"/>
+      <c r="AT47" s="36"/>
+      <c r="AU47" s="36"/>
+      <c r="AV47" s="36"/>
+      <c r="AW47" s="36"/>
+      <c r="AX47" s="36"/>
+      <c r="AY47" s="36"/>
+      <c r="AZ47" s="36"/>
+      <c r="BA47" s="36"/>
+      <c r="BB47" s="36"/>
+      <c r="BC47" s="36"/>
+      <c r="BD47" s="36"/>
+      <c r="BE47" s="36"/>
+      <c r="BF47" s="36"/>
+      <c r="BG47" s="36"/>
+      <c r="BH47" s="36"/>
+      <c r="BI47" s="36"/>
+      <c r="BJ47" s="36"/>
+      <c r="BK47" s="36"/>
+      <c r="BL47" s="36"/>
+      <c r="BM47" s="36"/>
+      <c r="BN47" s="36"/>
+      <c r="BO47" s="36"/>
     </row>
     <row r="48" spans="1:67" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48"/>
@@ -2681,7 +2738,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H9:J9 I6:BO6 L5:BO5 J7:BO7 H8:I8 L8:BO8 H25:BO46 H13:S13 H16:P16 H10:K12 X11:AH11 M11:V11 M9:W9 H15:V15 H14:U14 AA21:BO22 Z12:BO15 V12:Y12 AA16:BO19 H23:Z24 AJ9:AT11 AV9:BF11 BH9:BL11 BN9:BO11 Y9:AH10 AB23:BO24 AB20:BO20 H17:V18 H19:W22">
+  <conditionalFormatting sqref="L5:BO5 I6:BO6 J7:BO7 H8:I8 L8:BO8 H9:J9 M9:W9 Y9:AH10 AJ9:AT11 AV9:BF11 BH9:BL11 BN9:BO11 H10:K12 M11:V11 X11:AH11 V12:Y12 Z12:BO15 H13:S13 H14:U14 H15:V15 H16:P16 AA16:BO19 H17:V18 H19:W22 AB20:BO20 AA21:BO22 AB23:BO23 H23:Z24 AC24:BO24 BL25:BO25 H25:BI26 BK26:BO26 H27:BJ27 BL27:BO27 BK28:BO30 H28:BI32 H33:BL33 H34:BM35 H36:BN38 H39:BI39 H40:BN40 H41:BL41 H42:BK42 H43:BN46">
     <cfRule type="expression" dxfId="15" priority="9">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -2733,7 +2790,7 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="16">
+  <dataValidations disablePrompts="1" count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>